<commit_message>
update version name & version code.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/doc/CQLive适配清单.xlsx
+++ b/app/src/main/assets/doc/CQLive适配清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Source\CQLive\app\src\main\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB012C39-7427-407A-BF85-129A0D57E834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF8CAA8-9DFD-4FA7-A492-B9601780F7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,23 +117,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CQLive-TCL55A261-1.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-TCL55A261-1.15.apk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>企鹅极光1S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CQLive-PENGUIN1SA4062-1.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-PENGUIN1SA4062-1.15.apk</t>
+    <t>CQLive-PENGUIN1SA4062-1.18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.18.apk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-TCL55A261-1.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-TCL55A261-1.19.apk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,7 +522,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -600,10 +600,10 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K2" s="3"/>
     </row>
@@ -633,10 +633,10 @@
         <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K3" s="3"/>
     </row>

</xml_diff>

<commit_message>
set preload available time to 60s
</commit_message>
<xml_diff>
--- a/app/src/main/assets/doc/CQLive适配清单.xlsx
+++ b/app/src/main/assets/doc/CQLive适配清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Source\CQLive\app\src\main\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF8CAA8-9DFD-4FA7-A492-B9601780F7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F1958A-2379-4C38-9932-20B490003434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,19 +121,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CQLive-PENGUIN1SA4062-1.18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-PENGUIN1SA4062-1.18.apk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CQLive-TCL55A261-1.19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CQLive-TCL55A261-1.19.apk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.19.apk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,7 +522,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -600,10 +600,10 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2" s="3"/>
     </row>
@@ -633,10 +633,10 @@
         <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3"/>
     </row>

</xml_diff>

<commit_message>
update version name to 1.20.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/doc/CQLive适配清单.xlsx
+++ b/app/src/main/assets/doc/CQLive适配清单.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Source\CQLive\app\src\main\assets\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Src\outSource\CQLive\app\src\main\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF8CAA8-9DFD-4FA7-A492-B9601780F7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F92745-E512-4C3D-AB86-902F3B002736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,19 +121,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CQLive-PENGUIN1SA4062-1.18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-PENGUIN1SA4062-1.18.apk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-TCL55A261-1.19</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-TCL55A261-1.19.apk</t>
+    <t>CQLive-PENGUIN1SA4062-1.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.19.apk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-TCL55A261-1.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-TCL55A261-1.20.apk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,7 +522,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change MB to Mb.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/doc/CQLive适配清单.xlsx
+++ b/app/src/main/assets/doc/CQLive适配清单.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Source\CQLive\app\src\main\assets\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Src\outSource\CQLive\app\src\main\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FF2555-E7E2-4521-BBD7-FDE0D4FA5019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF50AF80-096D-4717-BAC5-E1A0DFAD8E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,19 +125,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CQLive-PENGUIN1SA4062-1.21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-PENGUIN1SA4062-1.21.apk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CQLive-TCL55A261-1.22.apk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CQLive-TCL55A261-1.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.23.apk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -526,7 +526,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -604,10 +604,10 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K2" s="3"/>
     </row>
@@ -637,10 +637,10 @@
         <v>24</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3"/>
     </row>

</xml_diff>

<commit_message>
add clock to project menu.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/doc/CQLive适配清单.xlsx
+++ b/app/src/main/assets/doc/CQLive适配清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Src\outSource\CQLive\app\src\main\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF50AF80-096D-4717-BAC5-E1A0DFAD8E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40644D8B-418F-4C1C-B3D7-3D1756DDDCDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,11 +133,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CQLive-PENGUIN1SA4062-1.23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CQLive-PENGUIN1SA4062-1.23.apk</t>
+    <t>CQLive-PENGUIN1SA4062-1.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQLive-PENGUIN1SA4062-1.24.apk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -526,7 +526,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix category/channel focus priority problem
</commit_message>
<xml_diff>
--- a/app/src/main/assets/doc/CQLive适配清单.xlsx
+++ b/app/src/main/assets/doc/CQLive适配清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Src\outSource\CQLive\app\src\main\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C2B493-ED38-4FB1-9CC7-A21E5A64FD19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DF2486-D101-4A3C-8531-4761BA202D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>适配设备</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +146,14 @@
   </si>
   <si>
     <t>线上版本1.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.26, 修复频道焦点优先级问题</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -207,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -230,11 +238,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -251,6 +270,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -531,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -546,13 +569,13 @@
     <col min="5" max="5" width="14.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
     <col min="9" max="9" width="31.6640625" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
     <col min="11" max="11" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -586,8 +609,11 @@
       <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L1" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -621,8 +647,11 @@
       <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="L2" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>